<commit_message>
TRA: remove linkages to external files; close #57
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_FT_Bounds.xlsx
+++ b/SuppXLS/Scen_TRA_FT_Bounds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D69B11-A3DD-4253-B26B-9D33309D1D0F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B539BF5D-97AF-482C-ADCC-946E73F7472E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,11 +20,6 @@
     <sheet name="Setup" sheetId="19" r:id="rId5"/>
     <sheet name="Conversions" sheetId="18" r:id="rId6"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId7"/>
-    <externalReference r:id="rId8"/>
-    <externalReference r:id="rId9"/>
-  </externalReferences>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="5" hidden="1">#REF!</definedName>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="3" hidden="1">#REF!</definedName>
@@ -128,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="240">
   <si>
     <t>Year</t>
   </si>
@@ -867,6 +862,9 @@
   <si>
     <t>*PJ</t>
   </si>
+  <si>
+    <t>UP</t>
+  </si>
 </sst>
 </file>
 
@@ -880,7 +878,7 @@
     <numFmt numFmtId="168" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="169" formatCode="#,##0.000000_);[Red]\(#,##0.000000\)"/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1058,12 +1056,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color indexed="8"/>
@@ -4298,7 +4290,7 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="27" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4390,368 +4382,6 @@
     <mc:Fallback/>
   </mc:AlternateContent>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Cover"/>
-      <sheetName val="Intro"/>
-      <sheetName val="EB2018"/>
-      <sheetName val="Regions"/>
-      <sheetName val="Commodities"/>
-      <sheetName val="Processes"/>
-      <sheetName val="FT"/>
-      <sheetName val="Stock"/>
-      <sheetName val="ACT2FLO"/>
-      <sheetName val="Demands"/>
-      <sheetName val="Efficiency"/>
-      <sheetName val="AF"/>
-      <sheetName val="On-Road Fac."/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3">
-        <row r="11">
-          <cell r="A11" t="str">
-            <v>IE-CW</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12" t="str">
-            <v>IE-CN</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13" t="str">
-            <v>IE-CE</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14" t="str">
-            <v>IE-CO</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15" t="str">
-            <v>IE-DL</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16" t="str">
-            <v>IE-D</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17" t="str">
-            <v>IE-G</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18" t="str">
-            <v>IE-KY</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="A19" t="str">
-            <v>IE-KE</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="A20" t="str">
-            <v>IE-KK</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="A21" t="str">
-            <v>IE-LS</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="A22" t="str">
-            <v>IE-LM</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="A23" t="str">
-            <v>IE-LK</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="A24" t="str">
-            <v>IE-LD</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="A25" t="str">
-            <v>IE-LH</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="A26" t="str">
-            <v>IE-MO</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="A27" t="str">
-            <v>IE-MH</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="A28" t="str">
-            <v>IE-MN</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="A29" t="str">
-            <v>IE-OY</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="A30" t="str">
-            <v>IE-RN</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="A31" t="str">
-            <v>IE-SO</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="A32" t="str">
-            <v>IE-TA</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="A33" t="str">
-            <v>IE-WD</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="A34" t="str">
-            <v>IE-WH</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="A35" t="str">
-            <v>IE-WX</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="A36" t="str">
-            <v>IE-WW</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Cover"/>
-      <sheetName val="Intro"/>
-      <sheetName val="EB2018"/>
-      <sheetName val="Regions"/>
-      <sheetName val="Commodities"/>
-      <sheetName val="Processes"/>
-      <sheetName val="FT"/>
-      <sheetName val="Stock"/>
-      <sheetName val="ACT2FLO"/>
-      <sheetName val="Demands"/>
-      <sheetName val="Efficiency"/>
-      <sheetName val="AF"/>
-      <sheetName val="On-Road Fac."/>
-      <sheetName val="Conversions"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3">
-        <row r="3">
-          <cell r="C3" t="str">
-            <v>IE</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="4">
-        <row r="6">
-          <cell r="C6" t="str">
-            <v>TRAWLK</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="5">
-        <row r="45">
-          <cell r="C45" t="str">
-            <v>IE,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Regions"/>
-      <sheetName val="config"/>
-      <sheetName val="single"/>
-      <sheetName val="multi"/>
-      <sheetName val="negative_CO2"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="4">
-          <cell r="B4" t="str">
-            <v>UC_N</v>
-          </cell>
-          <cell r="C4" t="str">
-            <v>UC_NetZero_CO2_2050</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="B5" t="str">
-            <v>UC_desc</v>
-          </cell>
-          <cell r="C5" t="str">
-            <v>Net Zero CO2 by 2050</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="B6" t="str">
-            <v>Year</v>
-          </cell>
-          <cell r="C6">
-            <v>2030</v>
-          </cell>
-          <cell r="D6">
-            <v>2050</v>
-          </cell>
-          <cell r="E6">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="B7" t="str">
-            <v>Value</v>
-          </cell>
-          <cell r="C7">
-            <v>19600</v>
-          </cell>
-          <cell r="D7">
-            <v>0</v>
-          </cell>
-          <cell r="E7">
-            <v>5</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="B8" t="str">
-            <v>Pset_PN</v>
-          </cell>
-          <cell r="C8" t="str">
-            <v>T-A*INT*,T-NAV*</v>
-          </cell>
-          <cell r="D8" t="str">
-            <v>T-A*INT*,T-NAV*</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="B9" t="str">
-            <v>Cset_CN</v>
-          </cell>
-          <cell r="C9" t="str">
-            <v>*CO2*,-*CO2S</v>
-          </cell>
-          <cell r="D9" t="str">
-            <v>*CO2*,-*CO2S</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="B10" t="str">
-            <v>Cset_Set</v>
-          </cell>
-          <cell r="C10" t="str">
-            <v>ENV</v>
-          </cell>
-          <cell r="D10" t="str">
-            <v>ENV</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="B11" t="str">
-            <v>Other_indexes</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="B12" t="str">
-            <v>LimType</v>
-          </cell>
-          <cell r="C12" t="str">
-            <v>UP</v>
-          </cell>
-          <cell r="D12" t="str">
-            <v>UP</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="B13" t="str">
-            <v>UC_FLO</v>
-          </cell>
-          <cell r="C13">
-            <v>-1</v>
-          </cell>
-          <cell r="D13">
-            <v>-1</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="B14" t="str">
-            <v>UC_COMNET</v>
-          </cell>
-          <cell r="C14">
-            <v>1</v>
-          </cell>
-          <cell r="D14">
-            <v>1</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5098,7 +4728,7 @@
   <dimension ref="A3:AD37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -5263,107 +4893,107 @@
         <v>9</v>
       </c>
       <c r="E5" s="6" t="str">
-        <f>[1]Regions!A11</f>
+        <f>Regions!A11</f>
         <v>IE-CW</v>
       </c>
       <c r="F5" s="6" t="str">
-        <f>[1]Regions!A16</f>
+        <f>Regions!A16</f>
         <v>IE-D</v>
       </c>
       <c r="G5" s="6" t="str">
-        <f>[1]Regions!A19</f>
+        <f>Regions!A19</f>
         <v>IE-KE</v>
       </c>
       <c r="H5" s="6" t="str">
-        <f>[1]Regions!A20</f>
+        <f>Regions!A20</f>
         <v>IE-KK</v>
       </c>
       <c r="I5" s="6" t="str">
-        <f>[1]Regions!A21</f>
+        <f>Regions!A21</f>
         <v>IE-LS</v>
       </c>
       <c r="J5" s="6" t="str">
-        <f>[1]Regions!A24</f>
+        <f>Regions!A24</f>
         <v>IE-LD</v>
       </c>
       <c r="K5" s="6" t="str">
-        <f>[1]Regions!A25</f>
+        <f>Regions!A25</f>
         <v>IE-LH</v>
       </c>
       <c r="L5" s="6" t="str">
-        <f>[1]Regions!A27</f>
+        <f>Regions!A27</f>
         <v>IE-MH</v>
       </c>
       <c r="M5" s="6" t="str">
-        <f>[1]Regions!A29</f>
+        <f>Regions!A29</f>
         <v>IE-OY</v>
       </c>
       <c r="N5" s="6" t="str">
-        <f>[1]Regions!A34</f>
+        <f>Regions!A34</f>
         <v>IE-WH</v>
       </c>
       <c r="O5" s="6" t="str">
-        <f>[1]Regions!A35</f>
+        <f>Regions!A35</f>
         <v>IE-WX</v>
       </c>
       <c r="P5" s="6" t="str">
-        <f>[1]Regions!A36</f>
+        <f>Regions!A36</f>
         <v>IE-WW</v>
       </c>
       <c r="Q5" s="6" t="str">
-        <f>[1]Regions!A13</f>
+        <f>Regions!A13</f>
         <v>IE-CE</v>
       </c>
       <c r="R5" s="6" t="str">
-        <f>[1]Regions!A14</f>
+        <f>Regions!A14</f>
         <v>IE-CO</v>
       </c>
       <c r="S5" s="6" t="str">
-        <f>[1]Regions!A18</f>
+        <f>Regions!A18</f>
         <v>IE-KY</v>
       </c>
       <c r="T5" s="6" t="str">
-        <f>[1]Regions!A23</f>
+        <f>Regions!A23</f>
         <v>IE-LK</v>
       </c>
       <c r="U5" s="6" t="str">
-        <f>[1]Regions!A32</f>
+        <f>Regions!A32</f>
         <v>IE-TA</v>
       </c>
       <c r="V5" s="6" t="str">
-        <f>[1]Regions!A33</f>
+        <f>Regions!A33</f>
         <v>IE-WD</v>
       </c>
       <c r="W5" s="6" t="str">
-        <f>[1]Regions!A17</f>
+        <f>Regions!A17</f>
         <v>IE-G</v>
       </c>
       <c r="X5" s="6" t="str">
-        <f>[1]Regions!A22</f>
+        <f>Regions!A22</f>
         <v>IE-LM</v>
       </c>
       <c r="Y5" s="6" t="str">
-        <f>[1]Regions!A26</f>
+        <f>Regions!A26</f>
         <v>IE-MO</v>
       </c>
       <c r="Z5" s="6" t="str">
-        <f>[1]Regions!A30</f>
+        <f>Regions!A30</f>
         <v>IE-RN</v>
       </c>
       <c r="AA5" s="6" t="str">
-        <f>[1]Regions!A31</f>
+        <f>Regions!A31</f>
         <v>IE-SO</v>
       </c>
       <c r="AB5" s="6" t="str">
-        <f>[1]Regions!A12</f>
+        <f>Regions!A12</f>
         <v>IE-CN</v>
       </c>
       <c r="AC5" s="6" t="str">
-        <f>[1]Regions!A15</f>
+        <f>Regions!A15</f>
         <v>IE-DL</v>
       </c>
       <c r="AD5" s="6" t="str">
-        <f>[1]Regions!A28</f>
+        <f>Regions!A28</f>
         <v>IE-MN</v>
       </c>
     </row>
@@ -13537,7 +13167,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13621,9 +13251,8 @@
       <c r="D7">
         <v>2018</v>
       </c>
-      <c r="E7" t="str">
-        <f>VLOOKUP(E$5, [3]config!$B$4:$E$14,2,FALSE)</f>
-        <v>UP</v>
+      <c r="E7" t="s">
+        <v>239</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -13645,9 +13274,8 @@
       <c r="D8">
         <v>2030</v>
       </c>
-      <c r="E8" t="str">
-        <f>VLOOKUP(E$5, [3]config!$B$4:$E$14,2,FALSE)</f>
-        <v>UP</v>
+      <c r="E8" t="s">
+        <v>239</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -13665,9 +13293,8 @@
       <c r="D9">
         <v>2050</v>
       </c>
-      <c r="E9" t="str">
-        <f>VLOOKUP(E$5, [3]config!$B$4:$E$14,2,FALSE)</f>
-        <v>UP</v>
+      <c r="E9" t="s">
+        <v>239</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -13685,9 +13312,8 @@
       <c r="D10">
         <v>0</v>
       </c>
-      <c r="E10" t="str">
-        <f>VLOOKUP(E$5, [3]config!$B$4:$E$14,2,FALSE)</f>
-        <v>UP</v>
+      <c r="E10" t="s">
+        <v>239</v>
       </c>
       <c r="G10">
         <f>HLOOKUP(D10,Setup!$B$4:$F$11,MATCH(C10,Setup!$B$4:$B$11,0),FALSE)</f>
@@ -13706,9 +13332,8 @@
       <c r="D11">
         <v>2018</v>
       </c>
-      <c r="E11" t="str">
-        <f>VLOOKUP(E$5, [3]config!$B$4:$E$14,2,FALSE)</f>
-        <v>UP</v>
+      <c r="E11" t="s">
+        <v>239</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -13730,9 +13355,8 @@
       <c r="D12">
         <v>2030</v>
       </c>
-      <c r="E12" t="str">
-        <f>VLOOKUP(E$5, [3]config!$B$4:$E$14,2,FALSE)</f>
-        <v>UP</v>
+      <c r="E12" t="s">
+        <v>239</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -13750,9 +13374,8 @@
       <c r="D13">
         <v>2050</v>
       </c>
-      <c r="E13" t="str">
-        <f>VLOOKUP(E$5, [3]config!$B$4:$E$14,2,FALSE)</f>
-        <v>UP</v>
+      <c r="E13" t="s">
+        <v>239</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -13770,9 +13393,8 @@
       <c r="D14">
         <v>0</v>
       </c>
-      <c r="E14" t="str">
-        <f>VLOOKUP(E$5, [3]config!$B$4:$E$14,2,FALSE)</f>
-        <v>UP</v>
+      <c r="E14" t="s">
+        <v>239</v>
       </c>
       <c r="G14">
         <f>HLOOKUP(D14,Setup!$B$4:$F$11,MATCH(C14,Setup!$B$4:$B$11,0),FALSE)</f>
@@ -13791,9 +13413,8 @@
       <c r="D15">
         <v>2018</v>
       </c>
-      <c r="E15" t="str">
-        <f>VLOOKUP(E$5, [3]config!$B$4:$E$14,2,FALSE)</f>
-        <v>UP</v>
+      <c r="E15" t="s">
+        <v>239</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -13815,9 +13436,8 @@
       <c r="D16">
         <v>2030</v>
       </c>
-      <c r="E16" t="str">
-        <f>VLOOKUP(E$5, [3]config!$B$4:$E$14,2,FALSE)</f>
-        <v>UP</v>
+      <c r="E16" t="s">
+        <v>239</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -13835,9 +13455,8 @@
       <c r="D17">
         <v>2050</v>
       </c>
-      <c r="E17" t="str">
-        <f>VLOOKUP(E$5, [3]config!$B$4:$E$14,2,FALSE)</f>
-        <v>UP</v>
+      <c r="E17" t="s">
+        <v>239</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -13855,9 +13474,8 @@
       <c r="D18">
         <v>0</v>
       </c>
-      <c r="E18" t="str">
-        <f>VLOOKUP(E$5, [3]config!$B$4:$E$14,2,FALSE)</f>
-        <v>UP</v>
+      <c r="E18" t="s">
+        <v>239</v>
       </c>
       <c r="G18">
         <f>HLOOKUP(D18,Setup!$B$4:$F$11,MATCH(C18,Setup!$B$4:$B$11,0),FALSE)</f>
@@ -13876,9 +13494,8 @@
       <c r="D19">
         <v>2018</v>
       </c>
-      <c r="E19" t="str">
-        <f>VLOOKUP(E$5, [3]config!$B$4:$E$14,2,FALSE)</f>
-        <v>UP</v>
+      <c r="E19" t="s">
+        <v>239</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -13900,9 +13517,8 @@
       <c r="D20">
         <v>2030</v>
       </c>
-      <c r="E20" t="str">
-        <f>VLOOKUP(E$5, [3]config!$B$4:$E$14,2,FALSE)</f>
-        <v>UP</v>
+      <c r="E20" t="s">
+        <v>239</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -13920,9 +13536,8 @@
       <c r="D21">
         <v>2050</v>
       </c>
-      <c r="E21" t="str">
-        <f>VLOOKUP(E$5, [3]config!$B$4:$E$14,2,FALSE)</f>
-        <v>UP</v>
+      <c r="E21" t="s">
+        <v>239</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -13940,9 +13555,8 @@
       <c r="D22">
         <v>0</v>
       </c>
-      <c r="E22" t="str">
-        <f>VLOOKUP(E$5, [3]config!$B$4:$E$14,2,FALSE)</f>
-        <v>UP</v>
+      <c r="E22" t="s">
+        <v>239</v>
       </c>
       <c r="G22">
         <f>HLOOKUP(D22,Setup!$B$4:$F$11,MATCH(C22,Setup!$B$4:$B$11,0),FALSE)</f>
@@ -13961,9 +13575,8 @@
       <c r="D23">
         <v>2018</v>
       </c>
-      <c r="E23" t="str">
-        <f>VLOOKUP(E$5, [3]config!$B$4:$E$14,2,FALSE)</f>
-        <v>UP</v>
+      <c r="E23" t="s">
+        <v>239</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -13985,9 +13598,8 @@
       <c r="D24">
         <v>2030</v>
       </c>
-      <c r="E24" t="str">
-        <f>VLOOKUP(E$5, [3]config!$B$4:$E$14,2,FALSE)</f>
-        <v>UP</v>
+      <c r="E24" t="s">
+        <v>239</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -14005,9 +13617,8 @@
       <c r="D25">
         <v>2050</v>
       </c>
-      <c r="E25" t="str">
-        <f>VLOOKUP(E$5, [3]config!$B$4:$E$14,2,FALSE)</f>
-        <v>UP</v>
+      <c r="E25" t="s">
+        <v>239</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -14025,9 +13636,8 @@
       <c r="D26">
         <v>0</v>
       </c>
-      <c r="E26" t="str">
-        <f>VLOOKUP(E$5, [3]config!$B$4:$E$14,2,FALSE)</f>
-        <v>UP</v>
+      <c r="E26" t="s">
+        <v>239</v>
       </c>
       <c r="G26">
         <f>HLOOKUP(D26,Setup!$B$4:$F$11,MATCH(C26,Setup!$B$4:$B$11,0),FALSE)</f>
@@ -14046,9 +13656,8 @@
       <c r="D27">
         <v>2018</v>
       </c>
-      <c r="E27" t="str">
-        <f>VLOOKUP(E$5, [3]config!$B$4:$E$14,2,FALSE)</f>
-        <v>UP</v>
+      <c r="E27" t="s">
+        <v>239</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -14070,9 +13679,8 @@
       <c r="D28">
         <v>2030</v>
       </c>
-      <c r="E28" t="str">
-        <f>VLOOKUP(E$5, [3]config!$B$4:$E$14,2,FALSE)</f>
-        <v>UP</v>
+      <c r="E28" t="s">
+        <v>239</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -14090,9 +13698,8 @@
       <c r="D29">
         <v>2050</v>
       </c>
-      <c r="E29" t="str">
-        <f>VLOOKUP(E$5, [3]config!$B$4:$E$14,2,FALSE)</f>
-        <v>UP</v>
+      <c r="E29" t="s">
+        <v>239</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -14110,9 +13717,8 @@
       <c r="D30">
         <v>0</v>
       </c>
-      <c r="E30" t="str">
-        <f>VLOOKUP(E$5, [3]config!$B$4:$E$14,2,FALSE)</f>
-        <v>UP</v>
+      <c r="E30" t="s">
+        <v>239</v>
       </c>
       <c r="G30">
         <f>HLOOKUP(D30,Setup!$B$4:$F$11,MATCH(C30,Setup!$B$4:$B$11,0),FALSE)</f>
@@ -14130,7 +13736,7 @@
   <dimension ref="B3:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14302,7 +13908,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>

</xml_diff>